<commit_message>
fix locator value, update data, fix spacing on test suite, added screenshot for UAT Deal 5
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT05.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B70359-A518-4113-831D-65FA81A8C31E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB871B6A-96DE-45E0-A409-69BB99FD179D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="520">
   <si>
     <t>rowid</t>
   </si>
@@ -1101,351 +1101,351 @@
     <t>UAT5</t>
   </si>
   <si>
-    <t>UAT5_08102019111016</t>
-  </si>
-  <si>
-    <t>UAT508102019111016</t>
+    <t>UAT5_26082020153847</t>
+  </si>
+  <si>
+    <t>UAT526082020153847</t>
+  </si>
+  <si>
+    <t>FACILITY-A_26082020134923VQX</t>
+  </si>
+  <si>
+    <t>19-Dec-2011</t>
+  </si>
+  <si>
+    <t>Sales Group 1</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>HOOD</t>
+  </si>
+  <si>
+    <t>Hood,  Robin</t>
+  </si>
+  <si>
+    <t>%AU-OBU</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>LENDING</t>
+  </si>
+  <si>
+    <t>Lending,  Ops</t>
+  </si>
+  <si>
+    <t>GCP</t>
+  </si>
+  <si>
+    <t>General Corp Purpose</t>
+  </si>
+  <si>
+    <t>499,815,787.36</t>
+  </si>
+  <si>
+    <t>IT_COL</t>
+  </si>
+  <si>
+    <t>Sydney, Australia</t>
+  </si>
+  <si>
+    <t>BBSW - Mid</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Base Rate and Spread Only By Formula</t>
+  </si>
+  <si>
+    <t>(Base + Spread + RAC) * PCT</t>
+  </si>
+  <si>
+    <t>Modified Following Business Day</t>
+  </si>
+  <si>
+    <t>Start of next cycle</t>
+  </si>
+  <si>
+    <t>Start of next interest cycle</t>
+  </si>
+  <si>
+    <t>COMMONWEALTH BANK AU-DBU</t>
+  </si>
+  <si>
+    <t>RE_RES</t>
+  </si>
+  <si>
+    <t>Origination</t>
+  </si>
+  <si>
+    <t>124,605,140.61</t>
+  </si>
+  <si>
+    <t>Hold for Investment - Australia</t>
+  </si>
+  <si>
+    <t>Commonwealth Bank of Australia - DBU</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>FACILITY-B_08102019114949AGS</t>
+  </si>
+  <si>
+    <t>13,691,190.48</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>FACILITY-C_08102019115619IXL</t>
+  </si>
+  <si>
+    <t>22,912,744.60</t>
+  </si>
+  <si>
+    <t>Facility_NamePrefix</t>
+  </si>
+  <si>
+    <t>Facility_Type</t>
+  </si>
+  <si>
+    <t>Facility_ProposedCmtAmt</t>
+  </si>
+  <si>
+    <t>Facility_LimitChangeDecreaseAmount</t>
+  </si>
+  <si>
+    <t>Facility_LimitChangeRemainingAmount</t>
+  </si>
+  <si>
+    <t>Facility_LimitChangeDecreaseAmtSched</t>
+  </si>
+  <si>
+    <t>Facility_LimitChangeRemainingAmtSched</t>
+  </si>
+  <si>
+    <t>Facility_Currency</t>
+  </si>
+  <si>
+    <t>Facility_AgreementDate</t>
+  </si>
+  <si>
+    <t>Facility_EffectiveDate</t>
+  </si>
+  <si>
+    <t>Facility_ExpiryDate</t>
+  </si>
+  <si>
+    <t>Facility_MaturityDate</t>
+  </si>
+  <si>
+    <t>Facility_ServicingGroup</t>
+  </si>
+  <si>
+    <t>Facility_Customer</t>
+  </si>
+  <si>
+    <t>Facility_RiskType</t>
+  </si>
+  <si>
+    <t>Facility_LoanPurposeType</t>
+  </si>
+  <si>
+    <t>Facility_GlobalLimit</t>
+  </si>
+  <si>
+    <t>Facility_SGLocation</t>
+  </si>
+  <si>
+    <t>Facility_Borrower</t>
+  </si>
+  <si>
+    <t>Borrower_Currency</t>
+  </si>
+  <si>
+    <t>Facility_BorrowerMaturity</t>
+  </si>
+  <si>
+    <t>Facility_BorrowerSGName</t>
+  </si>
+  <si>
+    <t>Facility_BorrowerPercent</t>
+  </si>
+  <si>
+    <t>CurrencyLimit</t>
+  </si>
+  <si>
+    <t>Facility_SIC</t>
+  </si>
+  <si>
+    <t>Facility_OwningBranch</t>
+  </si>
+  <si>
+    <t>Facility_FundingDesk</t>
+  </si>
+  <si>
+    <t>Facility_ProcessingArea</t>
+  </si>
+  <si>
+    <t>CBA_UAT_05</t>
+  </si>
+  <si>
+    <t>FACILITY-A_</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>3,435,325.23</t>
+  </si>
+  <si>
+    <t>121,169,815.38</t>
+  </si>
+  <si>
+    <t>28-Nov-2018</t>
+  </si>
+  <si>
+    <t>31-Dec-2021</t>
+  </si>
+  <si>
+    <t>16-Dec-2011</t>
+  </si>
+  <si>
+    <t>Refinance of Existing CBA/BW Loan</t>
+  </si>
+  <si>
+    <t>FLOAT</t>
+  </si>
+  <si>
+    <t>100.000000%</t>
+  </si>
+  <si>
+    <t>8432 - AU / Technical And Further Education</t>
+  </si>
+  <si>
+    <t>Australian (Sydney)</t>
+  </si>
+  <si>
+    <t>Agency Australia</t>
+  </si>
+  <si>
+    <t>FACILITY-B_</t>
+  </si>
+  <si>
+    <t>FACILITY-C_</t>
+  </si>
+  <si>
+    <t>Interest_AddItem</t>
+  </si>
+  <si>
+    <t>Interest_OptionName</t>
+  </si>
+  <si>
+    <t>Interest_RateBasis</t>
+  </si>
+  <si>
+    <t>Interest_SpreadValue</t>
+  </si>
+  <si>
+    <t>Interest_BaseRateCode_Formula</t>
+  </si>
+  <si>
+    <t>Interest_BaseRateCode_SpreadVar</t>
+  </si>
+  <si>
+    <t>Interest_BaseRateCode</t>
+  </si>
+  <si>
+    <t>Penalty_Spread</t>
+  </si>
+  <si>
+    <t>Penalty_Status</t>
+  </si>
+  <si>
+    <t>MIS_Code</t>
+  </si>
+  <si>
+    <t>MIS_Value</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Actual/365</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>( BBSW  + Spread (Spread_Var%) ) X PCT (1)</t>
+  </si>
+  <si>
+    <t>Spread_Var</t>
+  </si>
+  <si>
+    <t>( BBSW  + Spread (1.7%) ) X PCT (1)</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>RPLIM</t>
+  </si>
+  <si>
+    <t>RPL_Y</t>
+  </si>
+  <si>
+    <t>Facility_RowID</t>
+  </si>
+  <si>
+    <t>Loan_Alias</t>
+  </si>
+  <si>
+    <t>Borrower_Name</t>
+  </si>
+  <si>
+    <t>Pricing_Option</t>
+  </si>
+  <si>
+    <t>Outstanding_Type</t>
+  </si>
+  <si>
+    <t>Outstanding_Currency</t>
+  </si>
+  <si>
+    <t>Loan_RequestedAmount</t>
+  </si>
+  <si>
+    <t>Loan_EffectiveDate</t>
+  </si>
+  <si>
+    <t>Loan_MaturityDate</t>
+  </si>
+  <si>
+    <t>Loan_RepricingDate</t>
+  </si>
+  <si>
+    <t>Loan_RepricingFrequency</t>
+  </si>
+  <si>
+    <t>Loan_BorrowerBaseRate</t>
+  </si>
+  <si>
+    <t>Loan_RepricingSingleCashflow</t>
+  </si>
+  <si>
+    <t>Remittance_Description</t>
   </si>
   <si>
     <t>FACILITY-A_08102019114315QEE</t>
   </si>
   <si>
-    <t>19-Dec-2011</t>
-  </si>
-  <si>
-    <t>Sales Group 1</t>
-  </si>
-  <si>
-    <t>1011956</t>
-  </si>
-  <si>
-    <t>RH</t>
-  </si>
-  <si>
-    <t>HOOD</t>
-  </si>
-  <si>
-    <t>Hood,  Robin</t>
-  </si>
-  <si>
-    <t>%DBU</t>
-  </si>
-  <si>
-    <t>OL</t>
-  </si>
-  <si>
-    <t>LENDING</t>
-  </si>
-  <si>
-    <t>Lending,  Ops</t>
-  </si>
-  <si>
-    <t>GCP</t>
-  </si>
-  <si>
-    <t>General Corp Purpose</t>
-  </si>
-  <si>
-    <t>499,815,787.36</t>
-  </si>
-  <si>
-    <t>IT_COL</t>
-  </si>
-  <si>
-    <t>Sydney, Australia</t>
-  </si>
-  <si>
-    <t>BBSW - Mid</t>
-  </si>
-  <si>
-    <t>Actual</t>
-  </si>
-  <si>
-    <t>Base Rate and Spread Only By Formula</t>
-  </si>
-  <si>
-    <t>(Base + Spread + RAC) * PCT</t>
-  </si>
-  <si>
-    <t>Modified Following Business Day</t>
-  </si>
-  <si>
-    <t>Start of next cycle</t>
-  </si>
-  <si>
-    <t>Start of next interest cycle</t>
-  </si>
-  <si>
-    <t>COMMONWEALTH BANK AU-DBU</t>
-  </si>
-  <si>
-    <t>RE_RES</t>
-  </si>
-  <si>
-    <t>Origination</t>
-  </si>
-  <si>
-    <t>124,605,140.61</t>
-  </si>
-  <si>
-    <t>Hold for Investment - Australia</t>
-  </si>
-  <si>
-    <t>Commonwealth Bank of Australia - DBU</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>FACILITY-B_08102019114949AGS</t>
-  </si>
-  <si>
-    <t>13,691,190.48</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>FACILITY-C_08102019115619IXL</t>
-  </si>
-  <si>
-    <t>22,912,744.60</t>
-  </si>
-  <si>
-    <t>Facility_NamePrefix</t>
-  </si>
-  <si>
-    <t>Facility_Type</t>
-  </si>
-  <si>
-    <t>Facility_ProposedCmtAmt</t>
-  </si>
-  <si>
-    <t>Facility_LimitChangeDecreaseAmount</t>
-  </si>
-  <si>
-    <t>Facility_LimitChangeRemainingAmount</t>
-  </si>
-  <si>
-    <t>Facility_LimitChangeDecreaseAmtSched</t>
-  </si>
-  <si>
-    <t>Facility_LimitChangeRemainingAmtSched</t>
-  </si>
-  <si>
-    <t>Facility_Currency</t>
-  </si>
-  <si>
-    <t>Facility_AgreementDate</t>
-  </si>
-  <si>
-    <t>Facility_EffectiveDate</t>
-  </si>
-  <si>
-    <t>Facility_ExpiryDate</t>
-  </si>
-  <si>
-    <t>Facility_MaturityDate</t>
-  </si>
-  <si>
-    <t>Facility_ServicingGroup</t>
-  </si>
-  <si>
-    <t>Facility_Customer</t>
-  </si>
-  <si>
-    <t>Facility_RiskType</t>
-  </si>
-  <si>
-    <t>Facility_LoanPurposeType</t>
-  </si>
-  <si>
-    <t>Facility_GlobalLimit</t>
-  </si>
-  <si>
-    <t>Facility_SGLocation</t>
-  </si>
-  <si>
-    <t>Facility_Borrower</t>
-  </si>
-  <si>
-    <t>Borrower_Currency</t>
-  </si>
-  <si>
-    <t>Facility_BorrowerMaturity</t>
-  </si>
-  <si>
-    <t>Facility_BorrowerSGName</t>
-  </si>
-  <si>
-    <t>Facility_BorrowerPercent</t>
-  </si>
-  <si>
-    <t>CurrencyLimit</t>
-  </si>
-  <si>
-    <t>Facility_SIC</t>
-  </si>
-  <si>
-    <t>Facility_OwningBranch</t>
-  </si>
-  <si>
-    <t>Facility_FundingDesk</t>
-  </si>
-  <si>
-    <t>Facility_ProcessingArea</t>
-  </si>
-  <si>
-    <t>CBA_UAT_05</t>
-  </si>
-  <si>
-    <t>FACILITY-A_</t>
-  </si>
-  <si>
-    <t>Term</t>
-  </si>
-  <si>
-    <t>3,435,325.23</t>
-  </si>
-  <si>
-    <t>121,169,815.38</t>
-  </si>
-  <si>
-    <t>28-Nov-2018</t>
-  </si>
-  <si>
-    <t>31-Dec-2021</t>
-  </si>
-  <si>
-    <t>16-Dec-2011</t>
-  </si>
-  <si>
-    <t>Refinance of Existing CBA/BW Loan</t>
-  </si>
-  <si>
-    <t>FLOAT</t>
-  </si>
-  <si>
-    <t>100.000000%</t>
-  </si>
-  <si>
-    <t>8432 - AU / Technical And Further Education</t>
-  </si>
-  <si>
-    <t>Australian (Sydney)</t>
-  </si>
-  <si>
-    <t>Agency Australia</t>
-  </si>
-  <si>
-    <t>FACILITY-B_</t>
-  </si>
-  <si>
-    <t>FACILITY-C_</t>
-  </si>
-  <si>
-    <t>Interest_AddItem</t>
-  </si>
-  <si>
-    <t>Interest_OptionName</t>
-  </si>
-  <si>
-    <t>Interest_RateBasis</t>
-  </si>
-  <si>
-    <t>Interest_SpreadValue</t>
-  </si>
-  <si>
-    <t>Interest_BaseRateCode_Formula</t>
-  </si>
-  <si>
-    <t>Interest_BaseRateCode_SpreadVar</t>
-  </si>
-  <si>
-    <t>Interest_BaseRateCode</t>
-  </si>
-  <si>
-    <t>Penalty_Spread</t>
-  </si>
-  <si>
-    <t>Penalty_Status</t>
-  </si>
-  <si>
-    <t>MIS_Code</t>
-  </si>
-  <si>
-    <t>MIS_Value</t>
-  </si>
-  <si>
-    <t>Option</t>
-  </si>
-  <si>
-    <t>Actual/365</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t>( BBSW  + Spread (Spread_Var%) ) X PCT (1)</t>
-  </si>
-  <si>
-    <t>Spread_Var</t>
-  </si>
-  <si>
-    <t>( BBSW  + Spread (1.7%) ) X PCT (1)</t>
-  </si>
-  <si>
-    <t>Off</t>
-  </si>
-  <si>
-    <t>RPLIM</t>
-  </si>
-  <si>
-    <t>RPL_Y</t>
-  </si>
-  <si>
-    <t>Facility_RowID</t>
-  </si>
-  <si>
-    <t>Loan_Alias</t>
-  </si>
-  <si>
-    <t>Borrower_Name</t>
-  </si>
-  <si>
-    <t>Pricing_Option</t>
-  </si>
-  <si>
-    <t>Outstanding_Type</t>
-  </si>
-  <si>
-    <t>Outstanding_Currency</t>
-  </si>
-  <si>
-    <t>Loan_RequestedAmount</t>
-  </si>
-  <si>
-    <t>Loan_EffectiveDate</t>
-  </si>
-  <si>
-    <t>Loan_MaturityDate</t>
-  </si>
-  <si>
-    <t>Loan_RepricingDate</t>
-  </si>
-  <si>
-    <t>Loan_RepricingFrequency</t>
-  </si>
-  <si>
-    <t>Loan_BorrowerBaseRate</t>
-  </si>
-  <si>
-    <t>Loan_RepricingSingleCashflow</t>
-  </si>
-  <si>
-    <t>Remittance_Description</t>
-  </si>
-  <si>
     <t>60000017</t>
   </si>
   <si>
@@ -1557,7 +1557,7 @@
     <t>2.1</t>
   </si>
   <si>
-    <t>SANSEERA ELECTRONICS LTD1011954</t>
+    <t>SANSEERA ELECTRONICS LTD 1914539</t>
   </si>
   <si>
     <t>Awaiting release</t>
@@ -2133,8 +2133,8 @@
   <dimension ref="A1:CP2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2534,8 +2534,8 @@
   </sheetPr>
   <dimension ref="A1:EE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3494,7 +3494,9 @@
   </sheetPr>
   <dimension ref="A1:BA4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView topLeftCell="AU1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AZ2" sqref="AZ2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3752,49 +3754,49 @@
         <v>360</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>361</v>
+        <v>46</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>215</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>364</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>299</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>215</v>
       </c>
       <c r="U2" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>299</v>
       </c>
       <c r="Y2" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="23" t="s">
         <v>370</v>
-      </c>
-      <c r="AA2" s="23" t="s">
-        <v>371</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>211</v>
@@ -3803,52 +3805,52 @@
         <v>249</v>
       </c>
       <c r="AD2" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="AI2" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="AM2" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="AL2" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="AP2" s="1" t="s">
         <v>215</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AR2" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="AT2" s="1">
         <v>100</v>
@@ -3857,19 +3859,19 @@
         <v>100</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AW2" s="1" t="s">
         <v>299</v>
       </c>
       <c r="AX2" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="AY2" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="BA2" s="1" t="s">
         <v>359</v>
@@ -3877,24 +3879,24 @@
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="AX3" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="AX4" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="AX4" s="1" t="s">
-        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3911,7 +3913,9 @@
   </sheetPr>
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3959,7 +3963,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>304</v>
@@ -3971,88 +3975,88 @@
         <v>310</v>
       </c>
       <c r="G1" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>395</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>396</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="L1" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="O1" s="24" t="s">
         <v>401</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>402</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>403</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="R1" s="24" t="s">
         <v>404</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="S1" s="28" t="s">
         <v>405</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>406</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>407</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>409</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="X1" s="29" t="s">
         <v>410</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="Y1" s="28" t="s">
         <v>411</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="Z1" s="28" t="s">
         <v>412</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>413</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AB1" s="28" t="s">
         <v>414</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AC1" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="AC1" s="28" t="s">
+      <c r="AD1" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="AE1" s="24" t="s">
         <v>416</v>
       </c>
-      <c r="AD1" s="28" t="s">
-        <v>409</v>
-      </c>
-      <c r="AE1" s="24" t="s">
+      <c r="AF1" s="24" t="s">
         <v>417</v>
       </c>
-      <c r="AF1" s="24" t="s">
+      <c r="AG1" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="AG1" s="24" t="s">
+      <c r="AH1" s="24" t="s">
         <v>419</v>
-      </c>
-      <c r="AH1" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.2">
@@ -4060,10 +4064,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>421</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>422</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>356</v>
@@ -4075,114 +4079,114 @@
         <v>240</v>
       </c>
       <c r="G2" s="30" t="s">
+        <v>422</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="I2" s="31" t="s">
         <v>423</v>
       </c>
-      <c r="H2" s="31" t="s">
-        <v>384</v>
-      </c>
-      <c r="I2" s="31" t="s">
+      <c r="J2" s="31" t="s">
         <v>424</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="K2" s="31" t="s">
         <v>425</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="L2" s="16" t="s">
         <v>426</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>427</v>
       </c>
       <c r="M2" s="16" t="s">
         <v>240</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="O2" s="16" t="s">
         <v>359</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="S2" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="T2" s="31" t="s">
         <v>255</v>
       </c>
       <c r="U2" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="V2" s="16" t="s">
         <v>429</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>430</v>
       </c>
       <c r="W2" s="16" t="s">
         <v>215</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>361</v>
+        <v>46</v>
       </c>
       <c r="Y2" s="16" t="s">
         <v>240</v>
       </c>
       <c r="Z2" s="16" t="s">
+        <v>429</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="AB2" s="16" t="s">
         <v>430</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>431</v>
       </c>
       <c r="AC2" s="16" t="s">
         <v>240</v>
       </c>
       <c r="AD2" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AE2" s="16" t="s">
+        <v>431</v>
+      </c>
+      <c r="AF2" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="AG2" s="16" t="s">
         <v>432</v>
       </c>
-      <c r="AF2" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="AG2" s="16" t="s">
+      <c r="AH2" s="16" t="s">
         <v>433</v>
-      </c>
-      <c r="AH2" s="16" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="3" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>356</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F3" s="31" t="s">
         <v>240</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I3" s="31"/>
       <c r="J3" s="31"/>
@@ -4191,93 +4195,93 @@
         <v>240</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>359</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="S3" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="T3" s="31" t="s">
         <v>255</v>
       </c>
       <c r="U3" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="V3" s="16" t="s">
         <v>429</v>
-      </c>
-      <c r="V3" s="16" t="s">
-        <v>430</v>
       </c>
       <c r="W3" s="16" t="s">
         <v>215</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>361</v>
+        <v>46</v>
       </c>
       <c r="Y3" s="16" t="s">
         <v>240</v>
       </c>
       <c r="Z3" s="16" t="s">
+        <v>429</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="AB3" s="16" t="s">
         <v>430</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB3" s="16" t="s">
-        <v>431</v>
       </c>
       <c r="AC3" s="16" t="s">
         <v>240</v>
       </c>
       <c r="AD3" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AE3" s="16" t="s">
+        <v>431</v>
+      </c>
+      <c r="AF3" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="AG3" s="16" t="s">
         <v>432</v>
       </c>
-      <c r="AF3" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="AG3" s="16" t="s">
+      <c r="AH3" s="16" t="s">
         <v>433</v>
-      </c>
-      <c r="AH3" s="16" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>356</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>240</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I4" s="31"/>
       <c r="J4" s="31"/>
@@ -4286,67 +4290,67 @@
         <v>240</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="O4" s="16" t="s">
         <v>359</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="S4" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="T4" s="31" t="s">
         <v>255</v>
       </c>
       <c r="U4" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="V4" s="16" t="s">
         <v>429</v>
-      </c>
-      <c r="V4" s="16" t="s">
-        <v>430</v>
       </c>
       <c r="W4" s="16" t="s">
         <v>215</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>361</v>
+        <v>46</v>
       </c>
       <c r="Y4" s="16" t="s">
         <v>240</v>
       </c>
       <c r="Z4" s="16" t="s">
+        <v>429</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="AB4" s="16" t="s">
         <v>430</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB4" s="16" t="s">
-        <v>431</v>
       </c>
       <c r="AC4" s="16" t="s">
         <v>240</v>
       </c>
       <c r="AD4" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AE4" s="16" t="s">
+        <v>431</v>
+      </c>
+      <c r="AF4" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="AG4" s="16" t="s">
         <v>432</v>
       </c>
-      <c r="AF4" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="AG4" s="16" t="s">
+      <c r="AH4" s="16" t="s">
         <v>433</v>
-      </c>
-      <c r="AH4" s="16" t="s">
-        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -4393,37 +4397,37 @@
         <v>306</v>
       </c>
       <c r="D1" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>437</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>438</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>439</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>440</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>441</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="34" t="s">
         <v>442</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="32" t="s">
         <v>443</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>444</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>445</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="N1" s="32" t="s">
         <v>446</v>
-      </c>
-      <c r="N1" s="32" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4431,131 +4435,131 @@
         <v>41</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>358</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>374</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="31" t="s">
         <v>449</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="H2" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="35" t="s">
+        <v>386</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="K2" s="35" t="s">
-        <v>387</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>388</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>374</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="31" t="s">
         <v>449</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="H3" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="35" t="s">
+        <v>386</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="K3" s="35" t="s">
-        <v>387</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>391</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>374</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="31" t="s">
         <v>449</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="H4" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="35" t="s">
+        <v>386</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="K4" s="35" t="s">
-        <v>387</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -4570,10 +4574,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4584,22 +4588,22 @@
     <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="25.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="24" style="1" customWidth="1"/>
-    <col min="17" max="17" width="30.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="22.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="17.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="24" style="1" customWidth="1"/>
+    <col min="18" max="18" width="30.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="22.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4610,55 +4614,58 @@
         <v>304</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>306</v>
       </c>
       <c r="F1" s="22" t="s">
+        <v>457</v>
+      </c>
+      <c r="G1" s="22" t="s">
         <v>458</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>459</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="J1" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="22" t="s">
         <v>469</v>
       </c>
-      <c r="R1" s="22" t="s">
-        <v>470</v>
-      </c>
-      <c r="S1" s="22" t="s">
+      <c r="T1" s="22" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
@@ -4672,52 +4679,52 @@
         <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>358</v>
+        <v>470</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>471</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>374</v>
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>215</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="M2" s="16" t="s">
-        <v>427</v>
-      </c>
       <c r="N2" s="16" t="s">
+        <v>426</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>474</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>477</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>239</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>299</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>478</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>478</v>
@@ -4744,12 +4751,15 @@
         <v>478</v>
       </c>
       <c r="AC2" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>353</v>
@@ -4761,52 +4771,52 @@
         <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>358</v>
+        <v>470</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>479</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>374</v>
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>215</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="L3" s="36" t="s">
         <v>480</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="M3" s="16" t="s">
-        <v>427</v>
-      </c>
       <c r="N3" s="16" t="s">
+        <v>426</v>
+      </c>
+      <c r="O3" s="16" t="s">
         <v>482</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>239</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>299</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>478</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>478</v>
@@ -4833,12 +4843,15 @@
         <v>478</v>
       </c>
       <c r="AC3" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>353</v>
@@ -4847,55 +4860,55 @@
         <v>356</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>483</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>374</v>
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>215</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="K4" s="36" t="s">
-        <v>389</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="36" t="s">
+        <v>388</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="M4" s="16" t="s">
-        <v>427</v>
-      </c>
       <c r="N4" s="16" t="s">
+        <v>426</v>
+      </c>
+      <c r="O4" s="16" t="s">
         <v>485</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>239</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>299</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>478</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>478</v>
@@ -4922,10 +4935,13 @@
         <v>478</v>
       </c>
       <c r="AC4" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>487</v>
       </c>
@@ -4936,55 +4952,55 @@
         <v>356</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>488</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>374</v>
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>215</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="L5" s="36" t="s">
         <v>489</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="M5" s="16" t="s">
-        <v>427</v>
-      </c>
       <c r="N5" s="16" t="s">
+        <v>426</v>
+      </c>
+      <c r="O5" s="16" t="s">
         <v>474</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>239</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>299</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>478</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>478</v>
@@ -5011,6 +5027,9 @@
         <v>478</v>
       </c>
       <c r="AC5" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5073,10 +5092,10 @@
         <v>490</v>
       </c>
       <c r="F1" s="39" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H1" s="40" t="s">
         <v>491</v>
@@ -5097,7 +5116,7 @@
         <v>496</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="O1" s="42" t="s">
         <v>312</v>
@@ -5115,7 +5134,7 @@
         <v>500</v>
       </c>
       <c r="T1" s="32" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="U1" s="39" t="s">
         <v>501</v>
@@ -5129,13 +5148,13 @@
         <v>41</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>356</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>358</v>
+        <v>470</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>255</v>
@@ -5144,7 +5163,7 @@
         <v>471</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H2" s="31" t="s">
         <v>503</v>
@@ -5163,10 +5182,10 @@
         <v>506</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>361</v>
+        <v>46</v>
       </c>
       <c r="P2" s="41" t="s">
         <v>299</v>
@@ -5181,7 +5200,7 @@
         <v>507</v>
       </c>
       <c r="T2" s="44" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="U2" t="s">
         <v>508</v>
@@ -5224,16 +5243,16 @@
     </row>
     <row r="3" spans="1:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>356</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>358</v>
+        <v>470</v>
       </c>
       <c r="E3" s="38" t="s">
         <v>255</v>
@@ -5242,7 +5261,7 @@
         <v>479</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H3" s="31" t="s">
         <v>510</v>
@@ -5263,10 +5282,10 @@
         <v>506</v>
       </c>
       <c r="N3" s="43" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>361</v>
+        <v>46</v>
       </c>
       <c r="P3" s="41" t="s">
         <v>299</v>
@@ -5281,7 +5300,7 @@
         <v>514</v>
       </c>
       <c r="T3" s="44" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="U3" t="s">
         <v>508</v>
@@ -5324,16 +5343,16 @@
     </row>
     <row r="4" spans="1:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>356</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>255</v>
@@ -5342,13 +5361,13 @@
         <v>483</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H4" s="36" t="s">
         <v>515</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J4" s="36" t="s">
         <v>515</v>
@@ -5363,10 +5382,10 @@
         <v>506</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>361</v>
+        <v>46</v>
       </c>
       <c r="P4" s="41" t="s">
         <v>299</v>
@@ -5381,7 +5400,7 @@
         <v>518</v>
       </c>
       <c r="T4" s="44" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="U4" t="s">
         <v>508</v>
@@ -5427,13 +5446,13 @@
         <v>487</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>356</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E5" s="38" t="s">
         <v>255</v>
@@ -5442,10 +5461,10 @@
         <v>488</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I5" s="36" t="s">
         <v>489</v>
@@ -5461,10 +5480,10 @@
         <v>506</v>
       </c>
       <c r="N5" s="43" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>361</v>
+        <v>46</v>
       </c>
       <c r="P5" s="41" t="s">
         <v>299</v>
@@ -5479,7 +5498,7 @@
         <v>476</v>
       </c>
       <c r="T5" s="44" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="U5" t="s">
         <v>508</v>

</xml_diff>

<commit_message>
GDE-6759 Update Excel file
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT05.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT05.xlsx
@@ -3,13 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B776C168-1E21-4338-B47C-FE3B93364FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmamaril\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC157383-5C44-41E5-AFE1-929CED868152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="29070" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
-    <sheet name="ORIG03_Customer" sheetId="2" r:id="rId2"/>
+    <sheet name="PTY001_QuickPartyOnboarding" sheetId="8" r:id="rId1"/>
+    <sheet name="ORIG03_Customer" sheetId="9" r:id="rId2"/>
     <sheet name="CRED01_DealSetup" sheetId="3" r:id="rId3"/>
     <sheet name="CRED02_FacilitySetup" sheetId="4" r:id="rId4"/>
     <sheet name="CRED08_FacilityFeeSetup" sheetId="5" r:id="rId5"/>
@@ -17,12 +22,11 @@
     <sheet name="SERV08C_ComprehensiveRepricing" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="524">
   <si>
     <t>rowid</t>
   </si>
@@ -153,7 +157,7 @@
     <t>Create Quick Party Onboarding for CBA UAT Deal 2 - PTY001</t>
   </si>
   <si>
-    <t>Sanseera Electronics Ltd 1511713</t>
+    <t>Sanseera Electronics Ltd 1914539</t>
   </si>
   <si>
     <t>Yes</t>
@@ -162,7 +166,7 @@
     <t>Sanseera Electronics Ltd</t>
   </si>
   <si>
-    <t>1511713</t>
+    <t>1914539</t>
   </si>
   <si>
     <t>BEPTYLTDATFDANCESWITHWOLV</t>
@@ -740,7 +744,7 @@
     <t>High Value Local RTGS (AUD)</t>
   </si>
   <si>
-    <t>RTGS-AUD2521</t>
+    <t>RTGS-AUD2525</t>
   </si>
   <si>
     <t>AUD</t>
@@ -1094,351 +1098,354 @@
     <t>UAT5</t>
   </si>
   <si>
-    <t>UAT5_08102019111016</t>
-  </si>
-  <si>
-    <t>UAT508102019111016</t>
+    <t>UAT5_27082020152822</t>
+  </si>
+  <si>
+    <t>UAT527082020152823</t>
+  </si>
+  <si>
+    <t>FACILITY-A_27082020153340QNT</t>
+  </si>
+  <si>
+    <t>19-Dec-2011</t>
+  </si>
+  <si>
+    <t>Sales Group 1</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>HOOD</t>
+  </si>
+  <si>
+    <t>Hood,  Robin</t>
+  </si>
+  <si>
+    <t>%AU-OBU</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>LENDING</t>
+  </si>
+  <si>
+    <t>Lending,  Ops</t>
+  </si>
+  <si>
+    <t>GCP</t>
+  </si>
+  <si>
+    <t>General Corp Purpose</t>
+  </si>
+  <si>
+    <t>499,815,787.36</t>
+  </si>
+  <si>
+    <t>IT_COL</t>
+  </si>
+  <si>
+    <t>Sydney, Australia</t>
+  </si>
+  <si>
+    <t>BBSW - Mid</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Base Rate and Spread Only By Formula</t>
+  </si>
+  <si>
+    <t>(Base + Spread + RAC) * PCT</t>
+  </si>
+  <si>
+    <t>Modified Following Business Day</t>
+  </si>
+  <si>
+    <t>Start of next cycle</t>
+  </si>
+  <si>
+    <t>Start of next interest cycle</t>
+  </si>
+  <si>
+    <t>COMMONWEALTH BANK AU-OBU</t>
+  </si>
+  <si>
+    <t>RE_RES</t>
+  </si>
+  <si>
+    <t>Origination</t>
+  </si>
+  <si>
+    <t>124,605,140.61</t>
+  </si>
+  <si>
+    <t>Hold for Investment - Australia</t>
+  </si>
+  <si>
+    <t>Commonwealth Bank of Australia - OBU</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>FACILITY-B_08102019114949AGS</t>
+  </si>
+  <si>
+    <t>13,691,190.48</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>FACILITY-C_08102019115619IXL</t>
+  </si>
+  <si>
+    <t>22,912,744.60</t>
+  </si>
+  <si>
+    <t>Facility_NamePrefix</t>
+  </si>
+  <si>
+    <t>Facility_Type</t>
+  </si>
+  <si>
+    <t>Facility_ProposedCmtAmt</t>
+  </si>
+  <si>
+    <t>Facility_LimitChangeDecreaseAmount</t>
+  </si>
+  <si>
+    <t>Facility_LimitChangeRemainingAmount</t>
+  </si>
+  <si>
+    <t>Facility_LimitChangeDecreaseAmtSched</t>
+  </si>
+  <si>
+    <t>Facility_LimitChangeRemainingAmtSched</t>
+  </si>
+  <si>
+    <t>Facility_Currency</t>
+  </si>
+  <si>
+    <t>Facility_AgreementDate</t>
+  </si>
+  <si>
+    <t>Facility_EffectiveDate</t>
+  </si>
+  <si>
+    <t>Facility_ExpiryDate</t>
+  </si>
+  <si>
+    <t>Facility_MaturityDate</t>
+  </si>
+  <si>
+    <t>Facility_ServicingGroup</t>
+  </si>
+  <si>
+    <t>Facility_Customer</t>
+  </si>
+  <si>
+    <t>Facility_RiskType</t>
+  </si>
+  <si>
+    <t>Facility_LoanPurposeType</t>
+  </si>
+  <si>
+    <t>Facility_GlobalLimit</t>
+  </si>
+  <si>
+    <t>Facility_SGLocation</t>
+  </si>
+  <si>
+    <t>Facility_Borrower</t>
+  </si>
+  <si>
+    <t>Borrower_Currency</t>
+  </si>
+  <si>
+    <t>Facility_BorrowerMaturity</t>
+  </si>
+  <si>
+    <t>Facility_BorrowerSGName</t>
+  </si>
+  <si>
+    <t>Facility_BorrowerPercent</t>
+  </si>
+  <si>
+    <t>CurrencyLimit</t>
+  </si>
+  <si>
+    <t>Facility_SIC</t>
+  </si>
+  <si>
+    <t>Facility_OwningBranch</t>
+  </si>
+  <si>
+    <t>Facility_FundingDesk</t>
+  </si>
+  <si>
+    <t>Facility_ProcessingArea</t>
+  </si>
+  <si>
+    <t>CBA_UAT_05</t>
+  </si>
+  <si>
+    <t>FACILITY-A_</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>3,435,325.23</t>
+  </si>
+  <si>
+    <t>121,169,815.38</t>
+  </si>
+  <si>
+    <t>28-Nov-2018</t>
+  </si>
+  <si>
+    <t>31-Dec-2021</t>
+  </si>
+  <si>
+    <t>16-Dec-2011</t>
+  </si>
+  <si>
+    <t>Refinance of Existing CBA/BW Loan</t>
+  </si>
+  <si>
+    <t>FLOAT</t>
+  </si>
+  <si>
+    <t>100.000000%</t>
+  </si>
+  <si>
+    <t>8432 - AU / Technical And Further Education</t>
+  </si>
+  <si>
+    <t>Commonwealth Bank of Australia - DBU</t>
+  </si>
+  <si>
+    <t>Australian (Sydney)</t>
+  </si>
+  <si>
+    <t>Agency Australia</t>
+  </si>
+  <si>
+    <t>FACILITY-B_</t>
+  </si>
+  <si>
+    <t>FACILITY-C_</t>
+  </si>
+  <si>
+    <t>Interest_AddItem</t>
+  </si>
+  <si>
+    <t>Interest_OptionName</t>
+  </si>
+  <si>
+    <t>Interest_RateBasis</t>
+  </si>
+  <si>
+    <t>Interest_SpreadValue</t>
+  </si>
+  <si>
+    <t>Interest_BaseRateCode_Formula</t>
+  </si>
+  <si>
+    <t>Interest_BaseRateCode_SpreadVar</t>
+  </si>
+  <si>
+    <t>Interest_BaseRateCode</t>
+  </si>
+  <si>
+    <t>Penalty_Spread</t>
+  </si>
+  <si>
+    <t>Penalty_Status</t>
+  </si>
+  <si>
+    <t>MIS_Code</t>
+  </si>
+  <si>
+    <t>MIS_Value</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Actual/365</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>( BBSW  + Spread (Spread_Var%) ) X PCT (1)</t>
+  </si>
+  <si>
+    <t>Spread_Var</t>
+  </si>
+  <si>
+    <t>( BBSW  + Spread (1.7%) ) X PCT (1)</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>RPLIM</t>
+  </si>
+  <si>
+    <t>RPL_Y</t>
+  </si>
+  <si>
+    <t>Facility_RowID</t>
+  </si>
+  <si>
+    <t>Loan_Alias</t>
+  </si>
+  <si>
+    <t>Borrower_Name</t>
+  </si>
+  <si>
+    <t>Pricing_Option</t>
+  </si>
+  <si>
+    <t>Outstanding_Type</t>
+  </si>
+  <si>
+    <t>Outstanding_Currency</t>
+  </si>
+  <si>
+    <t>Loan_RequestedAmount</t>
+  </si>
+  <si>
+    <t>Loan_EffectiveDate</t>
+  </si>
+  <si>
+    <t>Loan_MaturityDate</t>
+  </si>
+  <si>
+    <t>Loan_RepricingDate</t>
+  </si>
+  <si>
+    <t>Loan_RepricingFrequency</t>
+  </si>
+  <si>
+    <t>Loan_BorrowerBaseRate</t>
+  </si>
+  <si>
+    <t>Loan_RepricingSingleCashflow</t>
+  </si>
+  <si>
+    <t>Remittance_Description</t>
   </si>
   <si>
     <t>FACILITY-A_08102019114315QEE</t>
   </si>
   <si>
-    <t>19-Dec-2011</t>
-  </si>
-  <si>
-    <t>Sales Group 1</t>
-  </si>
-  <si>
-    <t>1011956</t>
-  </si>
-  <si>
-    <t>RH</t>
-  </si>
-  <si>
-    <t>HOOD</t>
-  </si>
-  <si>
-    <t>Hood,  Robin</t>
-  </si>
-  <si>
-    <t>%DBU</t>
-  </si>
-  <si>
-    <t>OL</t>
-  </si>
-  <si>
-    <t>LENDING</t>
-  </si>
-  <si>
-    <t>Lending,  Ops</t>
-  </si>
-  <si>
-    <t>GCP</t>
-  </si>
-  <si>
-    <t>General Corp Purpose</t>
-  </si>
-  <si>
-    <t>499,815,787.36</t>
-  </si>
-  <si>
-    <t>IT_COL</t>
-  </si>
-  <si>
-    <t>Sydney, Australia</t>
-  </si>
-  <si>
-    <t>BBSW - Mid</t>
-  </si>
-  <si>
-    <t>Actual</t>
-  </si>
-  <si>
-    <t>Base Rate and Spread Only By Formula</t>
-  </si>
-  <si>
-    <t>(Base + Spread + RAC) * PCT</t>
-  </si>
-  <si>
-    <t>Modified Following Business Day</t>
-  </si>
-  <si>
-    <t>Start of next cycle</t>
-  </si>
-  <si>
-    <t>Start of next interest cycle</t>
-  </si>
-  <si>
-    <t>COMMONWEALTH BANK AU-DBU</t>
-  </si>
-  <si>
-    <t>RE_RES</t>
-  </si>
-  <si>
-    <t>Origination</t>
-  </si>
-  <si>
-    <t>124,605,140.61</t>
-  </si>
-  <si>
-    <t>Hold for Investment - Australia</t>
-  </si>
-  <si>
-    <t>Commonwealth Bank of Australia - DBU</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>FACILITY-B_08102019114949AGS</t>
-  </si>
-  <si>
-    <t>13,691,190.48</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>FACILITY-C_08102019115619IXL</t>
-  </si>
-  <si>
-    <t>22,912,744.60</t>
-  </si>
-  <si>
-    <t>Facility_NamePrefix</t>
-  </si>
-  <si>
-    <t>Facility_Type</t>
-  </si>
-  <si>
-    <t>Facility_ProposedCmtAmt</t>
-  </si>
-  <si>
-    <t>Facility_LimitChangeDecreaseAmount</t>
-  </si>
-  <si>
-    <t>Facility_LimitChangeRemainingAmount</t>
-  </si>
-  <si>
-    <t>Facility_LimitChangeDecreaseAmtSched</t>
-  </si>
-  <si>
-    <t>Facility_LimitChangeRemainingAmtSched</t>
-  </si>
-  <si>
-    <t>Facility_Currency</t>
-  </si>
-  <si>
-    <t>Facility_AgreementDate</t>
-  </si>
-  <si>
-    <t>Facility_EffectiveDate</t>
-  </si>
-  <si>
-    <t>Facility_ExpiryDate</t>
-  </si>
-  <si>
-    <t>Facility_MaturityDate</t>
-  </si>
-  <si>
-    <t>Facility_ServicingGroup</t>
-  </si>
-  <si>
-    <t>Facility_Customer</t>
-  </si>
-  <si>
-    <t>Facility_RiskType</t>
-  </si>
-  <si>
-    <t>Facility_LoanPurposeType</t>
-  </si>
-  <si>
-    <t>Facility_GlobalLimit</t>
-  </si>
-  <si>
-    <t>Facility_SGLocation</t>
-  </si>
-  <si>
-    <t>Facility_Borrower</t>
-  </si>
-  <si>
-    <t>Borrower_Currency</t>
-  </si>
-  <si>
-    <t>Facility_BorrowerMaturity</t>
-  </si>
-  <si>
-    <t>Facility_BorrowerSGName</t>
-  </si>
-  <si>
-    <t>Facility_BorrowerPercent</t>
-  </si>
-  <si>
-    <t>CurrencyLimit</t>
-  </si>
-  <si>
-    <t>Facility_SIC</t>
-  </si>
-  <si>
-    <t>Facility_OwningBranch</t>
-  </si>
-  <si>
-    <t>Facility_FundingDesk</t>
-  </si>
-  <si>
-    <t>Facility_ProcessingArea</t>
-  </si>
-  <si>
-    <t>CBA_UAT_05</t>
-  </si>
-  <si>
-    <t>FACILITY-A_</t>
-  </si>
-  <si>
-    <t>Term</t>
-  </si>
-  <si>
-    <t>3,435,325.23</t>
-  </si>
-  <si>
-    <t>121,169,815.38</t>
-  </si>
-  <si>
-    <t>28-Nov-2018</t>
-  </si>
-  <si>
-    <t>31-Dec-2021</t>
-  </si>
-  <si>
-    <t>16-Dec-2011</t>
-  </si>
-  <si>
-    <t>Refinance of Existing CBA/BW Loan</t>
-  </si>
-  <si>
-    <t>FLOAT</t>
-  </si>
-  <si>
-    <t>100.000000%</t>
-  </si>
-  <si>
-    <t>8432 - AU / Technical And Further Education</t>
-  </si>
-  <si>
-    <t>Australian (Sydney)</t>
-  </si>
-  <si>
-    <t>Agency Australia</t>
-  </si>
-  <si>
-    <t>FACILITY-B_</t>
-  </si>
-  <si>
-    <t>FACILITY-C_</t>
-  </si>
-  <si>
-    <t>Interest_AddItem</t>
-  </si>
-  <si>
-    <t>Interest_OptionName</t>
-  </si>
-  <si>
-    <t>Interest_RateBasis</t>
-  </si>
-  <si>
-    <t>Interest_SpreadValue</t>
-  </si>
-  <si>
-    <t>Interest_BaseRateCode_Formula</t>
-  </si>
-  <si>
-    <t>Interest_BaseRateCode_SpreadVar</t>
-  </si>
-  <si>
-    <t>Interest_BaseRateCode</t>
-  </si>
-  <si>
-    <t>Penalty_Spread</t>
-  </si>
-  <si>
-    <t>Penalty_Status</t>
-  </si>
-  <si>
-    <t>MIS_Code</t>
-  </si>
-  <si>
-    <t>MIS_Value</t>
-  </si>
-  <si>
-    <t>Option</t>
-  </si>
-  <si>
-    <t>Actual/365</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t>( BBSW  + Spread (Spread_Var%) ) X PCT (1)</t>
-  </si>
-  <si>
-    <t>Spread_Var</t>
-  </si>
-  <si>
-    <t>( BBSW  + Spread (1.7%) ) X PCT (1)</t>
-  </si>
-  <si>
-    <t>Off</t>
-  </si>
-  <si>
-    <t>RPLIM</t>
-  </si>
-  <si>
-    <t>RPL_Y</t>
-  </si>
-  <si>
-    <t>Facility_RowID</t>
-  </si>
-  <si>
-    <t>Loan_Alias</t>
-  </si>
-  <si>
-    <t>Borrower_Name</t>
-  </si>
-  <si>
-    <t>Pricing_Option</t>
-  </si>
-  <si>
-    <t>Outstanding_Type</t>
-  </si>
-  <si>
-    <t>Outstanding_Currency</t>
-  </si>
-  <si>
-    <t>Loan_RequestedAmount</t>
-  </si>
-  <si>
-    <t>Loan_EffectiveDate</t>
-  </si>
-  <si>
-    <t>Loan_MaturityDate</t>
-  </si>
-  <si>
-    <t>Loan_RepricingDate</t>
-  </si>
-  <si>
-    <t>Loan_RepricingFrequency</t>
-  </si>
-  <si>
-    <t>Loan_BorrowerBaseRate</t>
-  </si>
-  <si>
-    <t>Loan_RepricingSingleCashflow</t>
-  </si>
-  <si>
-    <t>Remittance_Description</t>
-  </si>
-  <si>
     <t>60000017</t>
   </si>
   <si>
@@ -1550,7 +1557,7 @@
     <t>2.1</t>
   </si>
   <si>
-    <t>SANSEERA ELECTRONICS LTD1011954</t>
+    <t>SANSEERA ELECTRONICS LTD 1914539</t>
   </si>
   <si>
     <t>Awaiting release</t>
@@ -1586,16 +1593,16 @@
     <t>167,154.30</t>
   </si>
   <si>
-    <t>Sanseera Electronics Ltd 1914539</t>
-  </si>
-  <si>
-    <t>1914539</t>
-  </si>
-  <si>
-    <t>RTGSAUD1-5803</t>
-  </si>
-  <si>
-    <t>RTGS-AUD2525</t>
+    <t>Sanseera Electronics Ltd 1511713</t>
+  </si>
+  <si>
+    <t>1511713</t>
+  </si>
+  <si>
+    <t>RTGSAUD1-5808</t>
+  </si>
+  <si>
+    <t>RTGS-AUD2521</t>
   </si>
 </sst>
 </file>
@@ -2131,7 +2138,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01205ECA-47EE-40D4-AA57-EDE111A2F9F8}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2410,7 +2417,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>520</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>44</v>
@@ -2419,7 +2426,7 @@
         <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>521</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>47</v>
@@ -2533,14 +2540,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA19861-75E9-40AE-A2FA-D27C0680C951}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:EE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN2" sqref="AN2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3090,13 +3097,13 @@
         <v>207</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>519</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>208</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>520</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>209</v>
@@ -3126,7 +3133,7 @@
         <v>217</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>520</v>
+        <v>46</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>218</v>
@@ -3201,10 +3208,10 @@
         <v>237</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AP2" s="1" t="s">
         <v>239</v>
@@ -3499,7 +3506,9 @@
   </sheetPr>
   <dimension ref="A1:BA4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3757,49 +3766,49 @@
         <v>359</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>360</v>
+        <v>46</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>215</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>298</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>215</v>
       </c>
       <c r="U2" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>367</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>298</v>
       </c>
       <c r="Y2" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="23" t="s">
         <v>369</v>
-      </c>
-      <c r="AA2" s="23" t="s">
-        <v>370</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>211</v>
@@ -3808,52 +3817,52 @@
         <v>248</v>
       </c>
       <c r="AD2" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="AI2" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="AM2" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="AL2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="AP2" s="1" t="s">
         <v>215</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AR2" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="AT2" s="1">
         <v>100</v>
@@ -3862,19 +3871,19 @@
         <v>100</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AW2" s="1" t="s">
         <v>298</v>
       </c>
       <c r="AX2" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="AY2" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="BA2" s="1" t="s">
         <v>358</v>
@@ -3882,24 +3891,24 @@
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="AX3" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="AX4" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="AX4" s="1" t="s">
-        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -3916,7 +3925,9 @@
   </sheetPr>
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3924,7 +3935,7 @@
     <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="38" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="57.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="24.7109375" style="1" customWidth="1"/>
@@ -3964,7 +3975,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>303</v>
@@ -3976,88 +3987,88 @@
         <v>309</v>
       </c>
       <c r="G1" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>393</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>395</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>396</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="L1" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="O1" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>401</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>402</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="R1" s="24" t="s">
         <v>403</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="S1" s="28" t="s">
         <v>404</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>405</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>406</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>407</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="X1" s="29" t="s">
         <v>409</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="Y1" s="28" t="s">
         <v>410</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="Z1" s="28" t="s">
         <v>411</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>412</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AB1" s="28" t="s">
         <v>413</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AC1" s="28" t="s">
         <v>414</v>
       </c>
-      <c r="AC1" s="28" t="s">
+      <c r="AD1" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="AE1" s="24" t="s">
         <v>415</v>
       </c>
-      <c r="AD1" s="28" t="s">
-        <v>408</v>
-      </c>
-      <c r="AE1" s="24" t="s">
+      <c r="AF1" s="24" t="s">
         <v>416</v>
       </c>
-      <c r="AF1" s="24" t="s">
+      <c r="AG1" s="24" t="s">
         <v>417</v>
       </c>
-      <c r="AG1" s="24" t="s">
+      <c r="AH1" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="AH1" s="24" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="2" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.2">
@@ -4065,10 +4076,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>420</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>421</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>355</v>
@@ -4080,82 +4091,82 @@
         <v>239</v>
       </c>
       <c r="G2" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>382</v>
+      </c>
+      <c r="I2" s="31" t="s">
         <v>422</v>
       </c>
-      <c r="H2" s="31" t="s">
-        <v>383</v>
-      </c>
-      <c r="I2" s="31" t="s">
+      <c r="J2" s="31" t="s">
         <v>423</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="K2" s="31" t="s">
         <v>424</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="L2" s="16" t="s">
         <v>425</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>426</v>
       </c>
       <c r="M2" s="16" t="s">
         <v>239</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="O2" s="16" t="s">
         <v>358</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S2" s="31" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="T2" s="31" t="s">
         <v>254</v>
       </c>
       <c r="U2" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="V2" s="16" t="s">
         <v>428</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>429</v>
       </c>
       <c r="W2" s="16" t="s">
         <v>215</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>360</v>
+        <v>46</v>
       </c>
       <c r="Y2" s="16" t="s">
         <v>239</v>
       </c>
       <c r="Z2" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AB2" s="16" t="s">
         <v>429</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>430</v>
       </c>
       <c r="AC2" s="16" t="s">
         <v>239</v>
       </c>
       <c r="AD2" s="16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AE2" s="16" t="s">
+        <v>430</v>
+      </c>
+      <c r="AF2" s="16" t="s">
         <v>431</v>
-      </c>
-      <c r="AF2" s="16" t="s">
-        <v>385</v>
       </c>
       <c r="AG2" s="16" t="s">
         <v>432</v>
@@ -4166,10 +4177,10 @@
     </row>
     <row r="3" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>434</v>
@@ -4178,16 +4189,16 @@
         <v>355</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F3" s="31" t="s">
         <v>239</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I3" s="31"/>
       <c r="J3" s="31"/>
@@ -4196,61 +4207,61 @@
         <v>239</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>358</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S3" s="31" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="T3" s="31" t="s">
         <v>254</v>
       </c>
       <c r="U3" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="V3" s="16" t="s">
         <v>428</v>
-      </c>
-      <c r="V3" s="16" t="s">
-        <v>429</v>
       </c>
       <c r="W3" s="16" t="s">
         <v>215</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>360</v>
+        <v>46</v>
       </c>
       <c r="Y3" s="16" t="s">
         <v>239</v>
       </c>
       <c r="Z3" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AB3" s="16" t="s">
         <v>429</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="AB3" s="16" t="s">
-        <v>430</v>
       </c>
       <c r="AC3" s="16" t="s">
         <v>239</v>
       </c>
       <c r="AD3" s="16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AE3" s="16" t="s">
+        <v>430</v>
+      </c>
+      <c r="AF3" s="16" t="s">
         <v>431</v>
-      </c>
-      <c r="AF3" s="16" t="s">
-        <v>385</v>
       </c>
       <c r="AG3" s="16" t="s">
         <v>432</v>
@@ -4261,10 +4272,10 @@
     </row>
     <row r="4" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C4" s="30" t="s">
         <v>435</v>
@@ -4273,16 +4284,16 @@
         <v>355</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>239</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I4" s="31"/>
       <c r="J4" s="31"/>
@@ -4291,61 +4302,61 @@
         <v>239</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="O4" s="16" t="s">
         <v>358</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S4" s="31" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="T4" s="31" t="s">
         <v>254</v>
       </c>
       <c r="U4" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="V4" s="16" t="s">
         <v>428</v>
-      </c>
-      <c r="V4" s="16" t="s">
-        <v>429</v>
       </c>
       <c r="W4" s="16" t="s">
         <v>215</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>360</v>
+        <v>46</v>
       </c>
       <c r="Y4" s="16" t="s">
         <v>239</v>
       </c>
       <c r="Z4" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AB4" s="16" t="s">
         <v>429</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="AB4" s="16" t="s">
-        <v>430</v>
       </c>
       <c r="AC4" s="16" t="s">
         <v>239</v>
       </c>
       <c r="AD4" s="16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AE4" s="16" t="s">
+        <v>430</v>
+      </c>
+      <c r="AF4" s="16" t="s">
         <v>431</v>
-      </c>
-      <c r="AF4" s="16" t="s">
-        <v>385</v>
       </c>
       <c r="AG4" s="16" t="s">
         <v>432</v>
@@ -4368,7 +4379,9 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4436,7 +4449,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>357</v>
@@ -4445,7 +4458,7 @@
         <v>447</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>448</v>
@@ -4463,7 +4476,7 @@
         <v>452</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>453</v>
@@ -4477,19 +4490,19 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>420</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>387</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>447</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>448</v>
@@ -4507,7 +4520,7 @@
         <v>452</v>
       </c>
       <c r="K3" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>453</v>
@@ -4521,19 +4534,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>420</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>390</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>447</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>448</v>
@@ -4551,7 +4564,7 @@
         <v>452</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>453</v>
@@ -4575,10 +4588,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4589,22 +4602,22 @@
     <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="25.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="24" style="1" customWidth="1"/>
-    <col min="17" max="17" width="30.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="22.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="17.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="24" style="1" customWidth="1"/>
+    <col min="18" max="18" width="30.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="22.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4627,43 +4640,46 @@
         <v>458</v>
       </c>
       <c r="H1" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>459</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="S1" s="22" t="s">
         <v>469</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="T1" s="22" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
@@ -4677,84 +4693,87 @@
         <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>357</v>
+        <v>470</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>373</v>
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>215</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="M2" s="16" t="s">
-        <v>426</v>
+      <c r="M2" s="1" t="s">
+        <v>473</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>473</v>
-      </c>
-      <c r="O2" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>474</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>476</v>
       </c>
       <c r="R2" t="s">
+        <v>477</v>
+      </c>
+      <c r="S2" t="s">
         <v>238</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>298</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>477</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AC2" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>352</v>
@@ -4766,37 +4785,37 @@
         <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>357</v>
+        <v>470</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>373</v>
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>215</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="K3" s="36" t="s">
-        <v>479</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="36" t="s">
         <v>480</v>
       </c>
-      <c r="M3" s="16" t="s">
-        <v>426</v>
+      <c r="M3" s="1" t="s">
+        <v>481</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>481</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>474</v>
+        <v>425</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>482</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>475</v>
@@ -4804,46 +4823,49 @@
       <c r="Q3" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="S3" t="s">
         <v>238</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>298</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>477</v>
-      </c>
       <c r="U3" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AC3" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>352</v>
@@ -4852,87 +4874,90 @@
         <v>355</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>215</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="L4" s="36" t="s">
         <v>387</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>388</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>426</v>
+      <c r="M4" s="1" t="s">
+        <v>484</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>484</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>474</v>
+        <v>425</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>485</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="R4" t="s">
+        <v>486</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="S4" t="s">
         <v>238</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>298</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>477</v>
-      </c>
       <c r="U4" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AC4" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>352</v>
@@ -4941,39 +4966,39 @@
         <v>355</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>390</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>373</v>
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>215</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="K5" s="36" t="s">
-        <v>488</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>426</v>
+      <c r="L5" s="36" t="s">
+        <v>489</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>473</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>473</v>
-      </c>
-      <c r="O5" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="O5" s="16" t="s">
         <v>474</v>
       </c>
       <c r="P5" s="1" t="s">
@@ -4982,40 +5007,43 @@
       <c r="Q5" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="S5" t="s">
         <v>238</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>298</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>477</v>
-      </c>
       <c r="U5" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AC5" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5075,31 +5103,31 @@
         <v>305</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F1" s="39" t="s">
         <v>457</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="N1" s="37" t="s">
         <v>459</v>
@@ -5108,25 +5136,25 @@
         <v>311</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="Q1" s="39" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="R1" s="37" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="S1" s="37" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="T1" s="32" t="s">
         <v>439</v>
       </c>
       <c r="U1" s="39" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="V1" s="37" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="2" spans="1:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -5134,44 +5162,44 @@
         <v>41</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>355</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>357</v>
+        <v>470</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>254</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="J2" s="36" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="K2" s="36" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="L2" s="36"/>
       <c r="M2" s="38" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N2" s="43" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>360</v>
+        <v>46</v>
       </c>
       <c r="P2" s="41" t="s">
         <v>298</v>
@@ -5183,16 +5211,16 @@
         <v>239</v>
       </c>
       <c r="S2" s="44" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="T2" s="44" t="s">
         <v>449</v>
       </c>
       <c r="U2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="V2" s="45" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
@@ -5229,49 +5257,49 @@
     </row>
     <row r="3" spans="1:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>355</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>357</v>
+        <v>470</v>
       </c>
       <c r="E3" s="38" t="s">
         <v>254</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="K3" s="36" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="L3" s="36" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="M3" s="38" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N3" s="43" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>360</v>
+        <v>46</v>
       </c>
       <c r="P3" s="41" t="s">
         <v>298</v>
@@ -5283,16 +5311,16 @@
         <v>239</v>
       </c>
       <c r="S3" s="44" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="T3" s="44" t="s">
         <v>449</v>
       </c>
       <c r="U3" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="V3" s="45" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -5329,49 +5357,49 @@
     </row>
     <row r="4" spans="1:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>355</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>254</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="M4" s="38" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>360</v>
+        <v>46</v>
       </c>
       <c r="P4" s="41" t="s">
         <v>298</v>
@@ -5383,16 +5411,16 @@
         <v>239</v>
       </c>
       <c r="S4" s="44" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="T4" s="44" t="s">
         <v>449</v>
       </c>
       <c r="U4" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="V4" s="45" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
@@ -5429,47 +5457,47 @@
     </row>
     <row r="5" spans="1:54" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>355</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E5" s="38" t="s">
         <v>254</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="L5" s="36"/>
       <c r="M5" s="38" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N5" s="43" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>360</v>
+        <v>46</v>
       </c>
       <c r="P5" s="41" t="s">
         <v>298</v>
@@ -5481,16 +5509,16 @@
         <v>239</v>
       </c>
       <c r="S5" s="44" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="T5" s="44" t="s">
         <v>449</v>
       </c>
       <c r="U5" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="V5" s="45" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>

</xml_diff>

<commit_message>
GDE-6863 Fixed script issue after merging
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT05.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT05.xlsx
@@ -2965,17 +2965,17 @@
       </c>
       <c r="E2" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="F2" s="45" t="inlineStr">
         <is>
-          <t>UAT504092020173922</t>
+          <t>UAT507092020114431</t>
         </is>
       </c>
       <c r="G2" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-A_04092020174548HWZ</t>
+          <t>FACILITY-A_07092020115134ZWO</t>
         </is>
       </c>
       <c r="H2" s="45" t="inlineStr">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="G3" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-B_04092020175200TYM</t>
+          <t>FACILITY-B_07092020115901PQX</t>
         </is>
       </c>
       <c r="AX3" s="45" t="inlineStr">
@@ -3230,7 +3230,7 @@
       </c>
       <c r="G4" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-C_04092020175813KPX</t>
+          <t>FACILITY-C_07092020120504VXK</t>
         </is>
       </c>
       <c r="AX4" s="45" t="inlineStr">
@@ -3486,12 +3486,12 @@
       </c>
       <c r="D2" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="E2" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-A_04092020174548HWZ</t>
+          <t>FACILITY-A_07092020115134ZWO</t>
         </is>
       </c>
       <c r="F2" s="30" t="inlineStr">
@@ -3658,12 +3658,12 @@
       </c>
       <c r="D3" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="E3" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-B_04092020175200TYM</t>
+          <t>FACILITY-B_07092020115901PQX</t>
         </is>
       </c>
       <c r="F3" s="30" t="inlineStr">
@@ -3813,12 +3813,12 @@
       </c>
       <c r="D4" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="E4" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-C_04092020175813KPX</t>
+          <t>FACILITY-C_07092020120504VXK</t>
         </is>
       </c>
       <c r="F4" s="30" t="inlineStr">
@@ -4071,7 +4071,7 @@
       </c>
       <c r="C2" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-A_04092020174548HWZ</t>
+          <t>FACILITY-A_07092020115134ZWO</t>
         </is>
       </c>
       <c r="D2" s="45" t="inlineStr">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="C3" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-B_04092020175200TYM</t>
+          <t>FACILITY-B_07092020115901PQX</t>
         </is>
       </c>
       <c r="D3" s="45" t="inlineStr">
@@ -4215,7 +4215,7 @@
       </c>
       <c r="C4" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-C_04092020175813KPX</t>
+          <t>FACILITY-C_07092020120504VXK</t>
         </is>
       </c>
       <c r="D4" s="45" t="inlineStr">
@@ -4432,7 +4432,7 @@
       </c>
       <c r="C2" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="D2" s="45" t="inlineStr">
@@ -4584,7 +4584,7 @@
       </c>
       <c r="C3" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="D3" s="45" t="inlineStr">
@@ -4594,12 +4594,12 @@
       </c>
       <c r="E3" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-A_04092020174548HWZ</t>
+          <t>FACILITY-A_07092020115134ZWO</t>
         </is>
       </c>
       <c r="F3" s="45" t="inlineStr">
         <is>
-          <t>60000006</t>
+          <t>60000667</t>
         </is>
       </c>
       <c r="G3" s="45" t="inlineStr">
@@ -4736,7 +4736,7 @@
       </c>
       <c r="C4" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="D4" s="45" t="inlineStr">
@@ -4746,12 +4746,12 @@
       </c>
       <c r="E4" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-B_04092020175200TYM</t>
+          <t>FACILITY-B_07092020115901PQX</t>
         </is>
       </c>
       <c r="F4" s="45" t="inlineStr">
         <is>
-          <t>60000008</t>
+          <t>60000668</t>
         </is>
       </c>
       <c r="G4" s="45" t="inlineStr">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="C5" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="D5" s="45" t="inlineStr">
@@ -5195,7 +5195,7 @@
       </c>
       <c r="C2" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="D2" s="45" t="inlineStr">
@@ -5335,12 +5335,12 @@
       </c>
       <c r="C3" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="D3" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-A_04092020174548HWZ</t>
+          <t>FACILITY-A_07092020115134ZWO</t>
         </is>
       </c>
       <c r="E3" s="37" t="inlineStr">
@@ -5350,7 +5350,7 @@
       </c>
       <c r="F3" s="45" t="inlineStr">
         <is>
-          <t>60000006</t>
+          <t>60000667</t>
         </is>
       </c>
       <c r="G3" s="30" t="inlineStr">
@@ -5479,12 +5479,12 @@
       </c>
       <c r="C4" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="D4" s="45" t="inlineStr">
         <is>
-          <t>FACILITY-B_04092020175200TYM</t>
+          <t>FACILITY-B_07092020115901PQX</t>
         </is>
       </c>
       <c r="E4" s="37" t="inlineStr">
@@ -5494,7 +5494,7 @@
       </c>
       <c r="F4" s="45" t="inlineStr">
         <is>
-          <t>60000008</t>
+          <t>60000668</t>
         </is>
       </c>
       <c r="G4" s="30" t="inlineStr">
@@ -5623,7 +5623,7 @@
       </c>
       <c r="C5" s="45" t="inlineStr">
         <is>
-          <t>UAT5_04092020173921</t>
+          <t>UAT5_07092020114431</t>
         </is>
       </c>
       <c r="D5" s="45" t="inlineStr">

</xml_diff>